<commit_message>
clean analysResults and resultCalibration
</commit_message>
<xml_diff>
--- a/module/calibration/resultCalibration.xlsx
+++ b/module/calibration/resultCalibration.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sarah.bauduin\Documents\GitHub\appendix_lynxIBM\module\calibration\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{034F861E-4C7D-4B71-94A6-9877B963F4A9}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8AE6493B-EFD7-4F5D-B727-A6EE271D84A6}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="18285" windowHeight="6540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="11">
   <si>
     <t>pMortRes</t>
   </si>
@@ -55,18 +55,6 @@
   </si>
   <si>
     <t>Values to match</t>
-  </si>
-  <si>
-    <t>meanDisp Alps</t>
-  </si>
-  <si>
-    <t>medianDispAlps</t>
-  </si>
-  <si>
-    <t>meanDispJura</t>
-  </si>
-  <si>
-    <t>medianDispJura</t>
   </si>
   <si>
     <t>pRepro</t>
@@ -421,10 +409,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:O13"/>
+  <dimension ref="A1:K13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L7" sqref="L7"/>
+      <selection activeCell="N11" sqref="N11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -439,14 +427,10 @@
     <col min="8" max="8" width="11.5703125" style="2" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="8.28515625" style="2" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="9" style="2" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="14.140625" style="2" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="15.42578125" style="2" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="13.42578125" style="2" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="15.140625" style="2" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="11.42578125" style="2"/>
+    <col min="11" max="11" width="11.42578125" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" s="5" t="s">
         <v>9</v>
       </c>
@@ -463,22 +447,10 @@
         <v>0.28999999999999998</v>
       </c>
       <c r="K1" s="4">
-        <v>27</v>
-      </c>
-      <c r="L1" s="4">
-        <v>20.6</v>
-      </c>
-      <c r="M1" s="4">
-        <v>29.5</v>
-      </c>
-      <c r="N1" s="4">
-        <v>33</v>
-      </c>
-      <c r="O1" s="4">
         <v>0.81</v>
       </c>
     </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>8</v>
       </c>
@@ -495,7 +467,7 @@
         <v>3</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="G2" s="2" t="s">
         <v>7</v>
@@ -512,20 +484,8 @@
       <c r="K2" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="L2" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="M2" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="N2" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="O2" s="2" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>1</v>
       </c>
@@ -557,22 +517,10 @@
         <v>0.6373837</v>
       </c>
       <c r="K3" s="2">
-        <v>26.606000000000002</v>
-      </c>
-      <c r="L3" s="2">
-        <v>13.795</v>
-      </c>
-      <c r="M3" s="2">
-        <v>28.03</v>
-      </c>
-      <c r="N3" s="2">
-        <v>15.93</v>
-      </c>
-      <c r="O3" s="2">
         <v>0.64639999999999997</v>
       </c>
     </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>2</v>
       </c>
@@ -604,22 +552,10 @@
         <v>0.29383749999999997</v>
       </c>
       <c r="K4" s="2">
-        <v>24.96</v>
-      </c>
-      <c r="L4" s="2">
-        <v>15.11</v>
-      </c>
-      <c r="M4" s="2">
-        <v>26.49</v>
-      </c>
-      <c r="N4" s="2">
-        <v>18.079999999999998</v>
-      </c>
-      <c r="O4" s="2">
         <v>0.74070000000000003</v>
       </c>
     </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>3</v>
       </c>
@@ -651,22 +587,10 @@
         <v>0.2936318</v>
       </c>
       <c r="K5" s="2">
-        <v>25.83</v>
-      </c>
-      <c r="L5" s="2">
-        <v>15.52</v>
-      </c>
-      <c r="M5" s="2">
-        <v>26.5</v>
-      </c>
-      <c r="N5" s="2">
-        <v>18.399999999999999</v>
-      </c>
-      <c r="O5" s="2">
         <v>0.78639999999999999</v>
       </c>
     </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>4</v>
       </c>
@@ -698,22 +622,10 @@
         <v>0.28155419999999998</v>
       </c>
       <c r="K6" s="2">
-        <v>25.95</v>
-      </c>
-      <c r="L6" s="2">
-        <v>15.52</v>
-      </c>
-      <c r="M6" s="2">
-        <v>27.74</v>
-      </c>
-      <c r="N6" s="2">
-        <v>18.239999999999998</v>
-      </c>
-      <c r="O6" s="2">
         <v>0.83199999999999996</v>
       </c>
     </row>
-    <row r="7" spans="1:15" s="7" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:11" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A7" s="7">
         <v>5</v>
       </c>
@@ -745,42 +657,30 @@
         <v>0.28972389999999998</v>
       </c>
       <c r="K7" s="8">
-        <v>26.57</v>
-      </c>
-      <c r="L7" s="8">
-        <v>15.57</v>
-      </c>
-      <c r="M7" s="8">
-        <v>27.86</v>
-      </c>
-      <c r="N7" s="8">
-        <v>18.309999999999999</v>
-      </c>
-      <c r="O7" s="8">
         <v>0.81710000000000005</v>
       </c>
     </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B8" s="6"/>
       <c r="C8" s="6"/>
       <c r="D8" s="6"/>
       <c r="E8" s="6"/>
       <c r="F8" s="6"/>
     </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B10" s="6"/>
       <c r="C10" s="6"/>
       <c r="D10" s="6"/>
       <c r="E10" s="6"/>
       <c r="F10" s="6"/>
     </row>
-    <row r="11" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B11" s="6"/>
       <c r="C11" s="6"/>
       <c r="D11" s="6"/>
       <c r="E11" s="6"/>
     </row>
-    <row r="13" spans="1:15" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:11" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B13" s="1"/>
       <c r="C13" s="1"/>
       <c r="D13" s="1"/>
@@ -791,10 +691,6 @@
       <c r="I13" s="2"/>
       <c r="J13" s="2"/>
       <c r="K13" s="2"/>
-      <c r="L13" s="2"/>
-      <c r="M13" s="2"/>
-      <c r="N13" s="2"/>
-      <c r="O13" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>